<commit_message>
change tree hierarchy in constructor
</commit_message>
<xml_diff>
--- a/docs/new_rules_cha.xlsx
+++ b/docs/new_rules_cha.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\java\riskService\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7067C4-08C6-4C67-B799-ED232896A362}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27315" windowHeight="13260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="27318" windowHeight="13260" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="379">
   <si>
     <t>INN</t>
   </si>
@@ -1165,12 +1171,30 @@
   <si>
     <t>5410786860</t>
   </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1331,6 +1355,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1591,38 +1618,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JY40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="11.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.84765625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.59765625" style="16" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.34765625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="24" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.84765625" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="30" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.84765625" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="64" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="65" max="236" width="9.5" style="4" bestFit="1" customWidth="1"/>
     <col min="237" max="285" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="286" max="16384" width="10.875" style="4"/>
+    <col min="286" max="16384" width="10.84765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:285">
+    <row r="1" spans="1:285" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2479,7 +2506,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2" spans="1:285" s="8" customFormat="1">
+    <row r="2" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="5">
         <v>8602166992</v>
       </c>
@@ -3336,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:285" s="9" customFormat="1">
+    <row r="3" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A3" s="1">
         <v>8602166992</v>
       </c>
@@ -4193,7 +4220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:285" s="9" customFormat="1">
+    <row r="4" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A4" s="34" t="s">
         <v>371</v>
       </c>
@@ -5050,7 +5077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:285" s="9" customFormat="1">
+    <row r="5" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A5" s="1">
         <v>8602166992</v>
       </c>
@@ -5907,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:285" s="13" customFormat="1">
+    <row r="6" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A6" s="11">
         <v>8602166992</v>
       </c>
@@ -6764,7 +6791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:285" s="8" customFormat="1">
+    <row r="7" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A7" s="5">
         <v>5410786860</v>
       </c>
@@ -7621,7 +7648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:285" s="9" customFormat="1">
+    <row r="8" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A8" s="34" t="s">
         <v>372</v>
       </c>
@@ -8478,7 +8505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:285" s="9" customFormat="1">
+    <row r="9" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A9" s="1">
         <v>5410786860</v>
       </c>
@@ -9335,7 +9362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:285" s="13" customFormat="1">
+    <row r="10" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A10" s="11">
         <v>5410786860</v>
       </c>
@@ -10192,7 +10219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:285" s="8" customFormat="1">
+    <row r="11" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A11" s="5">
         <v>5503217263</v>
       </c>
@@ -11049,7 +11076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:285" s="9" customFormat="1">
+    <row r="12" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A12" s="1">
         <v>5503217263</v>
       </c>
@@ -11906,7 +11933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:285" s="9" customFormat="1">
+    <row r="13" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A13" s="1">
         <v>5503217263</v>
       </c>
@@ -12763,7 +12790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:285" s="13" customFormat="1">
+    <row r="14" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A14" s="11">
         <v>5503217263</v>
       </c>
@@ -13620,7 +13647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:285" s="8" customFormat="1">
+    <row r="15" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A15" s="5">
         <v>5402552025</v>
       </c>
@@ -14477,7 +14504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:285" s="9" customFormat="1">
+    <row r="16" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A16" s="1">
         <v>5402552025</v>
       </c>
@@ -15334,7 +15361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:285" s="9" customFormat="1">
+    <row r="17" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A17" s="1">
         <v>5402552025</v>
       </c>
@@ -16191,7 +16218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:285" s="9" customFormat="1">
+    <row r="18" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A18" s="1" t="s">
         <v>311</v>
       </c>
@@ -17048,7 +17075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:285" s="9" customFormat="1">
+    <row r="19" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A19" s="1">
         <v>5402552025</v>
       </c>
@@ -17905,7 +17932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:285" s="13" customFormat="1">
+    <row r="20" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A20" s="11">
         <v>5402552025</v>
       </c>
@@ -18762,7 +18789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:285" s="8" customFormat="1">
+    <row r="21" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A21" s="5">
         <v>3241012505</v>
       </c>
@@ -19619,7 +19646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:285" s="9" customFormat="1">
+    <row r="22" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A22" s="1">
         <v>3241012505</v>
       </c>
@@ -20476,7 +20503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:285" s="13" customFormat="1">
+    <row r="23" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A23" s="11">
         <v>3241012505</v>
       </c>
@@ -21333,7 +21360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:285" s="8" customFormat="1">
+    <row r="24" spans="1:285" s="8" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A24" s="5">
         <v>7451346741</v>
       </c>
@@ -22190,7 +22217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:285" s="9" customFormat="1">
+    <row r="25" spans="1:285" s="9" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A25" s="1">
         <v>7451346741</v>
       </c>
@@ -23047,7 +23074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:285" s="13" customFormat="1">
+    <row r="26" spans="1:285" s="13" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A26" s="11">
         <v>7451346741</v>
       </c>
@@ -23904,7 +23931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:285" s="23" customFormat="1">
+    <row r="27" spans="1:285" s="23" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A27" s="19">
         <v>5836603667</v>
       </c>
@@ -24761,7 +24788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:285" s="26" customFormat="1">
+    <row r="28" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A28" s="24">
         <v>5836603667</v>
       </c>
@@ -25618,7 +25645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:285" s="26" customFormat="1">
+    <row r="29" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A29" s="24">
         <v>5836603667</v>
       </c>
@@ -26475,7 +26502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:285" s="26" customFormat="1">
+    <row r="30" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A30" s="24">
         <v>5836603667</v>
       </c>
@@ -27332,7 +27359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:285" s="26" customFormat="1">
+    <row r="31" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A31" s="24">
         <v>5836603667</v>
       </c>
@@ -28189,7 +28216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:285" s="26" customFormat="1">
+    <row r="32" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A32" s="24">
         <v>5836603667</v>
       </c>
@@ -29046,7 +29073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:285" s="31" customFormat="1">
+    <row r="33" spans="1:285" s="31" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A33" s="28">
         <v>5836603667</v>
       </c>
@@ -29903,7 +29930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:285" s="26" customFormat="1">
+    <row r="34" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A34" s="24" t="s">
         <v>339</v>
       </c>
@@ -30760,7 +30787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:285" s="26" customFormat="1">
+    <row r="35" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A35" s="24" t="s">
         <v>339</v>
       </c>
@@ -31617,7 +31644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:285" s="26" customFormat="1">
+    <row r="36" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A36" s="24">
         <v>7705892352</v>
       </c>
@@ -32474,7 +32501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:285" s="26" customFormat="1">
+    <row r="37" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A37" s="24">
         <v>7705892352</v>
       </c>
@@ -33331,7 +33358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:285" s="26" customFormat="1">
+    <row r="38" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A38" s="24" t="s">
         <v>339</v>
       </c>
@@ -34188,7 +34215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:285" s="26" customFormat="1">
+    <row r="39" spans="1:285" s="26" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A39" s="24">
         <v>7705892352</v>
       </c>
@@ -35045,7 +35072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:285" s="31" customFormat="1">
+    <row r="40" spans="1:285" s="31" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A40" s="28">
         <v>7705892352</v>
       </c>
@@ -35909,19 +35936,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="3" max="3" width="127" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="18" customFormat="1">
+    <row r="1" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A1" s="17" t="s">
         <v>312</v>
       </c>
@@ -35956,7 +35983,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="18" customFormat="1">
+    <row r="2" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A2" s="18" t="s">
         <v>361</v>
       </c>
@@ -36002,7 +36029,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="18" customFormat="1">
+    <row r="3" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A3" s="18" t="s">
         <v>362</v>
       </c>
@@ -36046,7 +36073,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="18" customFormat="1">
+    <row r="4" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A4" s="18" t="s">
         <v>369</v>
       </c>
@@ -36099,111 +36126,129 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
         <v>364</v>
       </c>
       <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
         <v>365</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>366</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>368</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>374</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>375</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>377</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>370</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0</v>
       </c>
     </row>

</xml_diff>